<commit_message>
agregacion de documento de propuesta y cambios cronograma y agregacion de ruta para hacer documentacion de grado
</commit_message>
<xml_diff>
--- a/proyecto de grado LT/Cronograma Proyecto v1.xlsx
+++ b/proyecto de grado LT/Cronograma Proyecto v1.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{684FC945-7DAC-4870-8BF3-06A5ADA26E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -262,19 +263,19 @@
     <t>INICIO DEL PROYECTO</t>
   </si>
   <si>
-    <t>LACTOSOFT 2.0</t>
-  </si>
-  <si>
     <t>ACTIVIDADES:</t>
   </si>
   <si>
     <t>WILLIAM ENRIQUE MARTINEZ GOMEZ y CRISTIAN STIVEN GUERRERO ANDRADE</t>
+  </si>
+  <si>
+    <t>MAXIMIZANDO EL POTENCIAL ATLÉTICO: CIENCIA DE DATOS Y LACTATO EN EL DEPORTE DE ALTO RENDIMIENTO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -800,33 +801,17 @@
     <xf numFmtId="0" fontId="3" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="3" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="3" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -845,6 +830,22 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="3" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="3" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1119,637 +1120,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K45"/>
-  <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48:AO83"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" customWidth="1"/>
-    <col min="10" max="10" width="73.5703125" customWidth="1"/>
-    <col min="11" max="11" width="38.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="15" customHeight="1">
-      <c r="A1" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-    </row>
-    <row r="2" spans="1:11" ht="15" customHeight="1">
-      <c r="A2" s="42"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="J2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A3" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="14">
-        <v>7</v>
-      </c>
-      <c r="B4" s="15">
-        <v>8</v>
-      </c>
-      <c r="C4" s="16">
-        <v>9</v>
-      </c>
-      <c r="D4" s="15">
-        <v>10</v>
-      </c>
-      <c r="E4" s="16">
-        <v>11</v>
-      </c>
-      <c r="F4" s="15">
-        <v>12</v>
-      </c>
-      <c r="G4" s="17">
-        <v>13</v>
-      </c>
-      <c r="H4" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A5" s="18">
-        <v>14</v>
-      </c>
-      <c r="B5" s="19">
-        <v>15</v>
-      </c>
-      <c r="C5" s="20">
-        <v>16</v>
-      </c>
-      <c r="D5" s="19">
-        <v>17</v>
-      </c>
-      <c r="E5" s="20">
-        <v>18</v>
-      </c>
-      <c r="F5" s="19">
-        <v>19</v>
-      </c>
-      <c r="G5" s="21">
-        <v>20</v>
-      </c>
-      <c r="H5" s="43"/>
-      <c r="J5" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="14">
-        <v>21</v>
-      </c>
-      <c r="B6" s="15">
-        <v>22</v>
-      </c>
-      <c r="C6" s="16">
-        <v>23</v>
-      </c>
-      <c r="D6" s="15">
-        <v>24</v>
-      </c>
-      <c r="E6" s="16">
-        <v>25</v>
-      </c>
-      <c r="F6" s="15">
-        <v>26</v>
-      </c>
-      <c r="G6" s="17">
-        <v>27</v>
-      </c>
-      <c r="H6" s="43" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A7" s="18">
-        <v>29</v>
-      </c>
-      <c r="B7" s="19">
-        <v>30</v>
-      </c>
-      <c r="C7" s="20">
-        <v>1</v>
-      </c>
-      <c r="D7" s="19">
-        <v>2</v>
-      </c>
-      <c r="E7" s="20">
-        <v>3</v>
-      </c>
-      <c r="F7" s="19">
-        <v>4</v>
-      </c>
-      <c r="G7" s="21">
-        <v>5</v>
-      </c>
-      <c r="H7" s="43"/>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="42"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-    </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A9" s="42"/>
-      <c r="B9" s="42"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="14">
-        <v>6</v>
-      </c>
-      <c r="B10" s="15">
-        <v>7</v>
-      </c>
-      <c r="C10" s="16">
-        <v>8</v>
-      </c>
-      <c r="D10" s="15">
-        <v>9</v>
-      </c>
-      <c r="E10" s="16">
-        <v>10</v>
-      </c>
-      <c r="F10" s="15">
-        <v>11</v>
-      </c>
-      <c r="G10" s="17">
-        <v>12</v>
-      </c>
-      <c r="H10" s="43" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A11" s="18">
-        <v>13</v>
-      </c>
-      <c r="B11" s="19">
-        <v>14</v>
-      </c>
-      <c r="C11" s="20">
-        <v>15</v>
-      </c>
-      <c r="D11" s="19">
-        <v>16</v>
-      </c>
-      <c r="E11" s="20">
-        <v>17</v>
-      </c>
-      <c r="F11" s="19">
-        <v>18</v>
-      </c>
-      <c r="G11" s="21">
-        <v>19</v>
-      </c>
-      <c r="H11" s="43"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="42"/>
-      <c r="K11" s="42"/>
-    </row>
-    <row r="12" spans="1:11" ht="15" customHeight="1">
-      <c r="A12" s="14">
-        <v>20</v>
-      </c>
-      <c r="B12" s="15">
-        <v>21</v>
-      </c>
-      <c r="C12" s="16">
-        <v>22</v>
-      </c>
-      <c r="D12" s="15">
-        <v>23</v>
-      </c>
-      <c r="E12" s="16">
-        <v>24</v>
-      </c>
-      <c r="F12" s="15">
-        <v>25</v>
-      </c>
-      <c r="G12" s="17">
-        <v>26</v>
-      </c>
-      <c r="H12" s="43" t="s">
-        <v>26</v>
-      </c>
-      <c r="I12" s="42"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="42"/>
-    </row>
-    <row r="13" spans="1:11" ht="69.75" customHeight="1" thickBot="1">
-      <c r="A13" s="18">
-        <v>27</v>
-      </c>
-      <c r="B13" s="19">
-        <v>28</v>
-      </c>
-      <c r="C13" s="20">
-        <v>29</v>
-      </c>
-      <c r="D13" s="19">
-        <v>30</v>
-      </c>
-      <c r="E13" s="20">
-        <v>31</v>
-      </c>
-      <c r="F13" s="19">
-        <v>1</v>
-      </c>
-      <c r="G13" s="21">
-        <v>2</v>
-      </c>
-      <c r="H13" s="43"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="8"/>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="42"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="10"/>
-    </row>
-    <row r="15" spans="1:11" ht="48.75" customHeight="1" thickBot="1">
-      <c r="A15" s="42"/>
-      <c r="B15" s="42"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-    </row>
-    <row r="16" spans="1:11" ht="75" customHeight="1" thickBot="1">
-      <c r="A16" s="4">
-        <v>3</v>
-      </c>
-      <c r="B16" s="5">
-        <v>4</v>
-      </c>
-      <c r="C16" s="6">
-        <v>5</v>
-      </c>
-      <c r="D16" s="5">
-        <v>6</v>
-      </c>
-      <c r="E16" s="6">
-        <v>7</v>
-      </c>
-      <c r="F16" s="5">
-        <v>8</v>
-      </c>
-      <c r="G16" s="7">
-        <v>9</v>
-      </c>
-      <c r="H16" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-    </row>
-    <row r="17" spans="9:11">
-      <c r="I17" s="9"/>
-    </row>
-    <row r="18" spans="9:11">
-      <c r="I18" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="J18" s="42"/>
-      <c r="K18" s="42"/>
-    </row>
-    <row r="19" spans="9:11">
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
-      <c r="K19" s="42"/>
-    </row>
-    <row r="20" spans="9:11" ht="60">
-      <c r="I20" s="9">
-        <v>1</v>
-      </c>
-      <c r="J20" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="K20" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="9:11">
-      <c r="I21" s="9">
-        <v>2</v>
-      </c>
-      <c r="J21" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="K21" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="9:11">
-      <c r="I22" s="9">
-        <v>3</v>
-      </c>
-      <c r="J22" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K22" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="9:11">
-      <c r="I23" s="9">
-        <v>4</v>
-      </c>
-      <c r="J23" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="K23" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="9:11">
-      <c r="I24" s="9">
-        <v>5</v>
-      </c>
-      <c r="J24" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="9:11">
-      <c r="I25" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="J25" s="42"/>
-      <c r="K25" s="42"/>
-    </row>
-    <row r="26" spans="9:11">
-      <c r="I26" s="42"/>
-      <c r="J26" s="42"/>
-      <c r="K26" s="42"/>
-    </row>
-    <row r="27" spans="9:11">
-      <c r="I27" s="9">
-        <v>1</v>
-      </c>
-      <c r="J27" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="K27" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="9:11">
-      <c r="I28" s="9">
-        <v>2</v>
-      </c>
-      <c r="J28" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="K28" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="9:11">
-      <c r="I29" s="9">
-        <v>3</v>
-      </c>
-      <c r="J29" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="K29" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="9:11">
-      <c r="I30" s="9">
-        <v>4</v>
-      </c>
-      <c r="J30" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="K30" s="9"/>
-    </row>
-    <row r="31" spans="9:11">
-      <c r="I31" s="9">
-        <v>5</v>
-      </c>
-      <c r="J31" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="32" spans="9:11">
-      <c r="I32" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="J32" s="42"/>
-      <c r="K32" s="42"/>
-    </row>
-    <row r="33" spans="9:11">
-      <c r="I33" s="42"/>
-      <c r="J33" s="42"/>
-      <c r="K33" s="42"/>
-    </row>
-    <row r="34" spans="9:11">
-      <c r="I34" s="9">
-        <v>1</v>
-      </c>
-      <c r="J34" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="K34" s="8"/>
-    </row>
-    <row r="35" spans="9:11">
-      <c r="I35" s="9">
-        <v>2</v>
-      </c>
-      <c r="J35" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="36" spans="9:11">
-      <c r="I36" s="9">
-        <v>3</v>
-      </c>
-      <c r="J36" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="K36" s="9"/>
-    </row>
-    <row r="37" spans="9:11">
-      <c r="I37" s="9">
-        <v>4</v>
-      </c>
-      <c r="J37" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="K37" s="9"/>
-    </row>
-    <row r="38" spans="9:11">
-      <c r="I38" s="9">
-        <v>5</v>
-      </c>
-      <c r="J38" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="9:11">
-      <c r="I39" s="42" t="s">
-        <v>43</v>
-      </c>
-      <c r="J39" s="42"/>
-      <c r="K39" s="42"/>
-    </row>
-    <row r="40" spans="9:11">
-      <c r="I40" s="42"/>
-      <c r="J40" s="42"/>
-      <c r="K40" s="42"/>
-    </row>
-    <row r="41" spans="9:11">
-      <c r="I41" s="9">
-        <v>1</v>
-      </c>
-      <c r="J41" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="K41" s="8"/>
-    </row>
-    <row r="42" spans="9:11">
-      <c r="I42" s="9">
-        <v>2</v>
-      </c>
-      <c r="J42" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="43" spans="9:11">
-      <c r="I43" s="9">
-        <v>3</v>
-      </c>
-      <c r="J43" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="K43" s="9"/>
-    </row>
-    <row r="44" spans="9:11">
-      <c r="I44" s="9">
-        <v>4</v>
-      </c>
-      <c r="J44" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="K44" s="9"/>
-    </row>
-    <row r="45" spans="9:11">
-      <c r="I45" s="9">
-        <v>5</v>
-      </c>
-      <c r="J45" t="s">
-        <v>45</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="I39:K40"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="A14:G15"/>
-    <mergeCell ref="I25:K26"/>
-    <mergeCell ref="I32:K33"/>
-    <mergeCell ref="A1:G2"/>
-    <mergeCell ref="I11:K12"/>
-    <mergeCell ref="I18:K19"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="A8:G9"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="K21" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:AQ43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:AP1"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1758,162 +1140,162 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:42" ht="16.5" thickBot="1">
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="47"/>
+      <c r="AA1" s="47"/>
+      <c r="AB1" s="47"/>
+      <c r="AC1" s="47"/>
+      <c r="AD1" s="47"/>
+      <c r="AE1" s="47"/>
+      <c r="AF1" s="47"/>
+      <c r="AG1" s="47"/>
+      <c r="AH1" s="47"/>
+      <c r="AI1" s="47"/>
+      <c r="AJ1" s="47"/>
+      <c r="AK1" s="47"/>
+      <c r="AL1" s="47"/>
+      <c r="AM1" s="47"/>
+      <c r="AN1" s="47"/>
+      <c r="AO1" s="47"/>
+      <c r="AP1" s="48"/>
+    </row>
+    <row r="2" spans="2:42">
+      <c r="B2" s="55" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55"/>
-      <c r="S1" s="55"/>
-      <c r="T1" s="55"/>
-      <c r="U1" s="55"/>
-      <c r="V1" s="55"/>
-      <c r="W1" s="55"/>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="55"/>
-      <c r="Z1" s="55"/>
-      <c r="AA1" s="55"/>
-      <c r="AB1" s="55"/>
-      <c r="AC1" s="55"/>
-      <c r="AD1" s="55"/>
-      <c r="AE1" s="55"/>
-      <c r="AF1" s="55"/>
-      <c r="AG1" s="55"/>
-      <c r="AH1" s="55"/>
-      <c r="AI1" s="55"/>
-      <c r="AJ1" s="55"/>
-      <c r="AK1" s="55"/>
-      <c r="AL1" s="55"/>
-      <c r="AM1" s="55"/>
-      <c r="AN1" s="55"/>
-      <c r="AO1" s="55"/>
-      <c r="AP1" s="56"/>
-    </row>
-    <row r="2" spans="2:42">
-      <c r="B2" s="47" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" s="50" t="s">
-        <v>79</v>
-      </c>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="45"/>
-      <c r="R2" s="45"/>
-      <c r="S2" s="45"/>
-      <c r="T2" s="45"/>
-      <c r="U2" s="45"/>
-      <c r="V2" s="45"/>
-      <c r="W2" s="45"/>
-      <c r="X2" s="45"/>
-      <c r="Y2" s="45"/>
-      <c r="Z2" s="45"/>
-      <c r="AA2" s="45"/>
-      <c r="AB2" s="45"/>
-      <c r="AC2" s="45"/>
-      <c r="AD2" s="45"/>
-      <c r="AE2" s="45"/>
-      <c r="AF2" s="45"/>
-      <c r="AG2" s="45"/>
-      <c r="AH2" s="45"/>
-      <c r="AI2" s="45"/>
-      <c r="AJ2" s="45"/>
-      <c r="AK2" s="45"/>
-      <c r="AL2" s="45"/>
-      <c r="AM2" s="45"/>
-      <c r="AN2" s="45"/>
-      <c r="AO2" s="45"/>
-      <c r="AP2" s="46"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="53"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="53"/>
+      <c r="U2" s="53"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
+      <c r="X2" s="53"/>
+      <c r="Y2" s="53"/>
+      <c r="Z2" s="53"/>
+      <c r="AA2" s="53"/>
+      <c r="AB2" s="53"/>
+      <c r="AC2" s="53"/>
+      <c r="AD2" s="53"/>
+      <c r="AE2" s="53"/>
+      <c r="AF2" s="53"/>
+      <c r="AG2" s="53"/>
+      <c r="AH2" s="53"/>
+      <c r="AI2" s="53"/>
+      <c r="AJ2" s="53"/>
+      <c r="AK2" s="53"/>
+      <c r="AL2" s="53"/>
+      <c r="AM2" s="53"/>
+      <c r="AN2" s="53"/>
+      <c r="AO2" s="53"/>
+      <c r="AP2" s="54"/>
     </row>
     <row r="3" spans="2:42">
-      <c r="B3" s="48"/>
-      <c r="C3" s="51">
-        <v>45139</v>
-      </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="51">
-        <v>45170</v>
-      </c>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="44">
-        <v>45200</v>
-      </c>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
-      <c r="N3" s="46"/>
-      <c r="O3" s="44">
-        <v>45231</v>
-      </c>
-      <c r="P3" s="45"/>
-      <c r="Q3" s="45"/>
-      <c r="R3" s="46"/>
-      <c r="S3" s="44">
-        <v>45261</v>
-      </c>
-      <c r="T3" s="45"/>
-      <c r="U3" s="45"/>
-      <c r="V3" s="46"/>
-      <c r="W3" s="44">
-        <v>45292</v>
-      </c>
-      <c r="X3" s="45"/>
-      <c r="Y3" s="45"/>
-      <c r="Z3" s="46"/>
-      <c r="AA3" s="44">
-        <v>45323</v>
-      </c>
-      <c r="AB3" s="45"/>
-      <c r="AC3" s="45"/>
-      <c r="AD3" s="46"/>
-      <c r="AE3" s="44">
-        <v>45352</v>
-      </c>
-      <c r="AF3" s="45"/>
-      <c r="AG3" s="45"/>
-      <c r="AH3" s="46"/>
-      <c r="AI3" s="44">
-        <v>45383</v>
-      </c>
-      <c r="AJ3" s="45"/>
-      <c r="AK3" s="45"/>
-      <c r="AL3" s="46"/>
-      <c r="AM3" s="44">
-        <v>45413</v>
-      </c>
-      <c r="AN3" s="45"/>
-      <c r="AO3" s="45"/>
-      <c r="AP3" s="46"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="59">
+        <v>44958</v>
+      </c>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="59">
+        <v>44986</v>
+      </c>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="52">
+        <v>45017</v>
+      </c>
+      <c r="L3" s="53"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="52">
+        <v>45047</v>
+      </c>
+      <c r="P3" s="53"/>
+      <c r="Q3" s="53"/>
+      <c r="R3" s="54"/>
+      <c r="S3" s="52">
+        <v>45078</v>
+      </c>
+      <c r="T3" s="53"/>
+      <c r="U3" s="53"/>
+      <c r="V3" s="54"/>
+      <c r="W3" s="52">
+        <v>45474</v>
+      </c>
+      <c r="X3" s="53"/>
+      <c r="Y3" s="53"/>
+      <c r="Z3" s="54"/>
+      <c r="AA3" s="52">
+        <v>45505</v>
+      </c>
+      <c r="AB3" s="53"/>
+      <c r="AC3" s="53"/>
+      <c r="AD3" s="54"/>
+      <c r="AE3" s="52">
+        <v>45536</v>
+      </c>
+      <c r="AF3" s="53"/>
+      <c r="AG3" s="53"/>
+      <c r="AH3" s="54"/>
+      <c r="AI3" s="52">
+        <v>45566</v>
+      </c>
+      <c r="AJ3" s="53"/>
+      <c r="AK3" s="53"/>
+      <c r="AL3" s="54"/>
+      <c r="AM3" s="52">
+        <v>45597</v>
+      </c>
+      <c r="AN3" s="53"/>
+      <c r="AO3" s="53"/>
+      <c r="AP3" s="54"/>
     </row>
     <row r="4" spans="2:42">
-      <c r="B4" s="49"/>
+      <c r="B4" s="57"/>
       <c r="C4" s="30">
         <v>1</v>
       </c>
@@ -3521,227 +2903,227 @@
       <c r="AP37" s="23"/>
     </row>
     <row r="38" spans="2:43" ht="15.75" thickBot="1">
-      <c r="B38" s="52"/>
+      <c r="B38" s="42"/>
     </row>
     <row r="39" spans="2:43" ht="15.75" thickBot="1">
-      <c r="B39" s="52"/>
-      <c r="C39" s="57"/>
-      <c r="D39" s="58"/>
-      <c r="E39" s="58"/>
-      <c r="F39" s="58"/>
-      <c r="G39" s="58"/>
-      <c r="H39" s="58"/>
-      <c r="I39" s="58"/>
-      <c r="J39" s="58"/>
-      <c r="K39" s="58"/>
-      <c r="L39" s="58"/>
-      <c r="M39" s="58"/>
-      <c r="N39" s="58"/>
-      <c r="O39" s="58"/>
-      <c r="P39" s="58"/>
-      <c r="Q39" s="58"/>
-      <c r="R39" s="58"/>
-      <c r="S39" s="58"/>
-      <c r="T39" s="58"/>
-      <c r="U39" s="58"/>
-      <c r="V39" s="58"/>
-      <c r="W39" s="58"/>
-      <c r="X39" s="58"/>
-      <c r="Y39" s="58"/>
-      <c r="Z39" s="58"/>
-      <c r="AA39" s="58"/>
-      <c r="AB39" s="58"/>
-      <c r="AC39" s="58"/>
-      <c r="AD39" s="58"/>
-      <c r="AE39" s="58"/>
-      <c r="AF39" s="58"/>
-      <c r="AG39" s="58"/>
-      <c r="AH39" s="58"/>
-      <c r="AI39" s="58"/>
-      <c r="AJ39" s="58"/>
-      <c r="AK39" s="58"/>
-      <c r="AL39" s="58"/>
-      <c r="AM39" s="58"/>
-      <c r="AN39" s="58"/>
-      <c r="AO39" s="58"/>
-      <c r="AP39" s="58"/>
-      <c r="AQ39" s="59"/>
+      <c r="B39" s="42"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="50"/>
+      <c r="E39" s="50"/>
+      <c r="F39" s="50"/>
+      <c r="G39" s="50"/>
+      <c r="H39" s="50"/>
+      <c r="I39" s="50"/>
+      <c r="J39" s="50"/>
+      <c r="K39" s="50"/>
+      <c r="L39" s="50"/>
+      <c r="M39" s="50"/>
+      <c r="N39" s="50"/>
+      <c r="O39" s="50"/>
+      <c r="P39" s="50"/>
+      <c r="Q39" s="50"/>
+      <c r="R39" s="50"/>
+      <c r="S39" s="50"/>
+      <c r="T39" s="50"/>
+      <c r="U39" s="50"/>
+      <c r="V39" s="50"/>
+      <c r="W39" s="50"/>
+      <c r="X39" s="50"/>
+      <c r="Y39" s="50"/>
+      <c r="Z39" s="50"/>
+      <c r="AA39" s="50"/>
+      <c r="AB39" s="50"/>
+      <c r="AC39" s="50"/>
+      <c r="AD39" s="50"/>
+      <c r="AE39" s="50"/>
+      <c r="AF39" s="50"/>
+      <c r="AG39" s="50"/>
+      <c r="AH39" s="50"/>
+      <c r="AI39" s="50"/>
+      <c r="AJ39" s="50"/>
+      <c r="AK39" s="50"/>
+      <c r="AL39" s="50"/>
+      <c r="AM39" s="50"/>
+      <c r="AN39" s="50"/>
+      <c r="AO39" s="50"/>
+      <c r="AP39" s="50"/>
+      <c r="AQ39" s="51"/>
     </row>
     <row r="40" spans="2:43" ht="15.75" thickBot="1">
-      <c r="B40" s="52"/>
-      <c r="C40" s="52"/>
-      <c r="D40" s="52"/>
-      <c r="E40" s="52"/>
-      <c r="F40" s="52"/>
-      <c r="G40" s="52"/>
-      <c r="H40" s="52"/>
-      <c r="I40" s="52"/>
-      <c r="J40" s="52"/>
-      <c r="K40" s="52"/>
-      <c r="L40" s="52"/>
-      <c r="M40" s="52"/>
-      <c r="N40" s="52"/>
-      <c r="O40" s="52"/>
-      <c r="P40" s="52"/>
-      <c r="Q40" s="52"/>
-      <c r="R40" s="52"/>
-      <c r="S40" s="52"/>
-      <c r="T40" s="52"/>
-      <c r="U40" s="52"/>
-      <c r="V40" s="52"/>
-      <c r="W40" s="52"/>
-      <c r="X40" s="52"/>
-      <c r="Y40" s="52"/>
-      <c r="Z40" s="52"/>
-      <c r="AA40" s="52"/>
-      <c r="AB40" s="52"/>
-      <c r="AC40" s="52"/>
-      <c r="AD40" s="52"/>
-      <c r="AE40" s="52"/>
-      <c r="AF40" s="52"/>
-      <c r="AG40" s="52"/>
-      <c r="AH40" s="52"/>
-      <c r="AI40" s="52"/>
-      <c r="AJ40" s="52"/>
-      <c r="AK40" s="52"/>
-      <c r="AL40" s="52"/>
-      <c r="AM40" s="52"/>
-      <c r="AN40" s="52"/>
-      <c r="AO40" s="52"/>
-      <c r="AP40" s="52"/>
-      <c r="AQ40" s="52"/>
+      <c r="B40" s="42"/>
+      <c r="C40" s="42"/>
+      <c r="D40" s="42"/>
+      <c r="E40" s="42"/>
+      <c r="F40" s="42"/>
+      <c r="G40" s="42"/>
+      <c r="H40" s="42"/>
+      <c r="I40" s="42"/>
+      <c r="J40" s="42"/>
+      <c r="K40" s="42"/>
+      <c r="L40" s="42"/>
+      <c r="M40" s="42"/>
+      <c r="N40" s="42"/>
+      <c r="O40" s="42"/>
+      <c r="P40" s="42"/>
+      <c r="Q40" s="42"/>
+      <c r="R40" s="42"/>
+      <c r="S40" s="42"/>
+      <c r="T40" s="42"/>
+      <c r="U40" s="42"/>
+      <c r="V40" s="42"/>
+      <c r="W40" s="42"/>
+      <c r="X40" s="42"/>
+      <c r="Y40" s="42"/>
+      <c r="Z40" s="42"/>
+      <c r="AA40" s="42"/>
+      <c r="AB40" s="42"/>
+      <c r="AC40" s="42"/>
+      <c r="AD40" s="42"/>
+      <c r="AE40" s="42"/>
+      <c r="AF40" s="42"/>
+      <c r="AG40" s="42"/>
+      <c r="AH40" s="42"/>
+      <c r="AI40" s="42"/>
+      <c r="AJ40" s="42"/>
+      <c r="AK40" s="42"/>
+      <c r="AL40" s="42"/>
+      <c r="AM40" s="42"/>
+      <c r="AN40" s="42"/>
+      <c r="AO40" s="42"/>
+      <c r="AP40" s="42"/>
+      <c r="AQ40" s="42"/>
     </row>
     <row r="41" spans="2:43" ht="15.75" thickBot="1">
-      <c r="B41" s="52"/>
-      <c r="C41" s="52"/>
-      <c r="D41" s="52"/>
-      <c r="E41" s="52"/>
-      <c r="F41" s="52"/>
-      <c r="G41" s="52"/>
-      <c r="H41" s="52"/>
-      <c r="I41" s="52"/>
-      <c r="J41" s="52"/>
-      <c r="K41" s="52"/>
-      <c r="L41" s="52"/>
-      <c r="M41" s="52"/>
-      <c r="N41" s="52"/>
-      <c r="O41" s="52"/>
-      <c r="P41" s="52"/>
-      <c r="Q41" s="52"/>
-      <c r="R41" s="52"/>
-      <c r="S41" s="52"/>
-      <c r="T41" s="52"/>
-      <c r="U41" s="52"/>
-      <c r="V41" s="52"/>
-      <c r="W41" s="52"/>
-      <c r="X41" s="52"/>
-      <c r="Y41" s="52"/>
-      <c r="Z41" s="52"/>
-      <c r="AA41" s="52"/>
-      <c r="AB41" s="52"/>
-      <c r="AC41" s="52"/>
-      <c r="AD41" s="52"/>
-      <c r="AE41" s="52"/>
-      <c r="AF41" s="52"/>
-      <c r="AG41" s="52"/>
-      <c r="AH41" s="52"/>
-      <c r="AI41" s="52"/>
-      <c r="AJ41" s="52"/>
-      <c r="AK41" s="52"/>
-      <c r="AL41" s="52"/>
-      <c r="AM41" s="52"/>
-      <c r="AN41" s="52"/>
-      <c r="AO41" s="52"/>
-      <c r="AP41" s="52"/>
-      <c r="AQ41" s="52"/>
+      <c r="B41" s="42"/>
+      <c r="C41" s="42"/>
+      <c r="D41" s="42"/>
+      <c r="E41" s="42"/>
+      <c r="F41" s="42"/>
+      <c r="G41" s="42"/>
+      <c r="H41" s="42"/>
+      <c r="I41" s="42"/>
+      <c r="J41" s="42"/>
+      <c r="K41" s="42"/>
+      <c r="L41" s="42"/>
+      <c r="M41" s="42"/>
+      <c r="N41" s="42"/>
+      <c r="O41" s="42"/>
+      <c r="P41" s="42"/>
+      <c r="Q41" s="42"/>
+      <c r="R41" s="42"/>
+      <c r="S41" s="42"/>
+      <c r="T41" s="42"/>
+      <c r="U41" s="42"/>
+      <c r="V41" s="42"/>
+      <c r="W41" s="42"/>
+      <c r="X41" s="42"/>
+      <c r="Y41" s="42"/>
+      <c r="Z41" s="42"/>
+      <c r="AA41" s="42"/>
+      <c r="AB41" s="42"/>
+      <c r="AC41" s="42"/>
+      <c r="AD41" s="42"/>
+      <c r="AE41" s="42"/>
+      <c r="AF41" s="42"/>
+      <c r="AG41" s="42"/>
+      <c r="AH41" s="42"/>
+      <c r="AI41" s="42"/>
+      <c r="AJ41" s="42"/>
+      <c r="AK41" s="42"/>
+      <c r="AL41" s="42"/>
+      <c r="AM41" s="42"/>
+      <c r="AN41" s="42"/>
+      <c r="AO41" s="42"/>
+      <c r="AP41" s="42"/>
+      <c r="AQ41" s="42"/>
     </row>
     <row r="42" spans="2:43" ht="15.75" thickBot="1">
-      <c r="B42" s="52"/>
-      <c r="C42" s="52"/>
-      <c r="D42" s="52"/>
-      <c r="E42" s="52"/>
-      <c r="F42" s="52"/>
-      <c r="G42" s="52"/>
-      <c r="H42" s="52"/>
-      <c r="I42" s="52"/>
-      <c r="J42" s="52"/>
-      <c r="K42" s="52"/>
-      <c r="L42" s="52"/>
-      <c r="M42" s="52"/>
-      <c r="N42" s="52"/>
-      <c r="O42" s="52"/>
-      <c r="P42" s="52"/>
-      <c r="Q42" s="52"/>
-      <c r="R42" s="52"/>
-      <c r="S42" s="52"/>
-      <c r="T42" s="52"/>
-      <c r="U42" s="52"/>
-      <c r="V42" s="52"/>
-      <c r="W42" s="52"/>
-      <c r="X42" s="52"/>
-      <c r="Y42" s="52"/>
-      <c r="Z42" s="52"/>
-      <c r="AA42" s="52"/>
-      <c r="AB42" s="52"/>
-      <c r="AC42" s="52"/>
-      <c r="AD42" s="52"/>
-      <c r="AE42" s="52"/>
-      <c r="AF42" s="52"/>
-      <c r="AG42" s="52"/>
-      <c r="AH42" s="52"/>
-      <c r="AI42" s="52"/>
-      <c r="AJ42" s="52"/>
-      <c r="AK42" s="52"/>
-      <c r="AL42" s="52"/>
-      <c r="AM42" s="52"/>
-      <c r="AN42" s="52"/>
-      <c r="AO42" s="52"/>
-      <c r="AP42" s="52"/>
-      <c r="AQ42" s="52"/>
+      <c r="B42" s="42"/>
+      <c r="C42" s="42"/>
+      <c r="D42" s="42"/>
+      <c r="E42" s="42"/>
+      <c r="F42" s="42"/>
+      <c r="G42" s="42"/>
+      <c r="H42" s="42"/>
+      <c r="I42" s="42"/>
+      <c r="J42" s="42"/>
+      <c r="K42" s="42"/>
+      <c r="L42" s="42"/>
+      <c r="M42" s="42"/>
+      <c r="N42" s="42"/>
+      <c r="O42" s="42"/>
+      <c r="P42" s="42"/>
+      <c r="Q42" s="42"/>
+      <c r="R42" s="42"/>
+      <c r="S42" s="42"/>
+      <c r="T42" s="42"/>
+      <c r="U42" s="42"/>
+      <c r="V42" s="42"/>
+      <c r="W42" s="42"/>
+      <c r="X42" s="42"/>
+      <c r="Y42" s="42"/>
+      <c r="Z42" s="42"/>
+      <c r="AA42" s="42"/>
+      <c r="AB42" s="42"/>
+      <c r="AC42" s="42"/>
+      <c r="AD42" s="42"/>
+      <c r="AE42" s="42"/>
+      <c r="AF42" s="42"/>
+      <c r="AG42" s="42"/>
+      <c r="AH42" s="42"/>
+      <c r="AI42" s="42"/>
+      <c r="AJ42" s="42"/>
+      <c r="AK42" s="42"/>
+      <c r="AL42" s="42"/>
+      <c r="AM42" s="42"/>
+      <c r="AN42" s="42"/>
+      <c r="AO42" s="42"/>
+      <c r="AP42" s="42"/>
+      <c r="AQ42" s="42"/>
     </row>
     <row r="43" spans="2:43" ht="15.75" thickBot="1">
-      <c r="B43" s="52"/>
-      <c r="C43" s="53"/>
-      <c r="D43" s="53"/>
-      <c r="E43" s="53"/>
-      <c r="F43" s="53"/>
-      <c r="G43" s="53"/>
-      <c r="H43" s="53"/>
-      <c r="I43" s="53"/>
-      <c r="J43" s="53"/>
-      <c r="K43" s="53"/>
-      <c r="L43" s="53"/>
-      <c r="M43" s="53"/>
-      <c r="N43" s="53"/>
-      <c r="O43" s="53"/>
-      <c r="P43" s="53"/>
-      <c r="Q43" s="53"/>
-      <c r="R43" s="53"/>
-      <c r="S43" s="53"/>
-      <c r="T43" s="53"/>
-      <c r="U43" s="53"/>
-      <c r="V43" s="53"/>
-      <c r="W43" s="53"/>
-      <c r="X43" s="53"/>
-      <c r="Y43" s="53"/>
-      <c r="Z43" s="53"/>
-      <c r="AA43" s="53"/>
-      <c r="AB43" s="53"/>
-      <c r="AC43" s="53"/>
-      <c r="AD43" s="53"/>
-      <c r="AE43" s="53"/>
-      <c r="AF43" s="53"/>
-      <c r="AG43" s="53"/>
-      <c r="AH43" s="53"/>
-      <c r="AI43" s="53"/>
-      <c r="AJ43" s="53"/>
-      <c r="AK43" s="53"/>
-      <c r="AL43" s="53"/>
-      <c r="AM43" s="53"/>
-      <c r="AN43" s="53"/>
-      <c r="AO43" s="53"/>
-      <c r="AP43" s="53"/>
-      <c r="AQ43" s="53"/>
+      <c r="B43" s="42"/>
+      <c r="C43" s="43"/>
+      <c r="D43" s="43"/>
+      <c r="E43" s="43"/>
+      <c r="F43" s="43"/>
+      <c r="G43" s="43"/>
+      <c r="H43" s="43"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="43"/>
+      <c r="K43" s="43"/>
+      <c r="L43" s="43"/>
+      <c r="M43" s="43"/>
+      <c r="N43" s="43"/>
+      <c r="O43" s="43"/>
+      <c r="P43" s="43"/>
+      <c r="Q43" s="43"/>
+      <c r="R43" s="43"/>
+      <c r="S43" s="43"/>
+      <c r="T43" s="43"/>
+      <c r="U43" s="43"/>
+      <c r="V43" s="43"/>
+      <c r="W43" s="43"/>
+      <c r="X43" s="43"/>
+      <c r="Y43" s="43"/>
+      <c r="Z43" s="43"/>
+      <c r="AA43" s="43"/>
+      <c r="AB43" s="43"/>
+      <c r="AC43" s="43"/>
+      <c r="AD43" s="43"/>
+      <c r="AE43" s="43"/>
+      <c r="AF43" s="43"/>
+      <c r="AG43" s="43"/>
+      <c r="AH43" s="43"/>
+      <c r="AI43" s="43"/>
+      <c r="AJ43" s="43"/>
+      <c r="AK43" s="43"/>
+      <c r="AL43" s="43"/>
+      <c r="AM43" s="43"/>
+      <c r="AN43" s="43"/>
+      <c r="AO43" s="43"/>
+      <c r="AP43" s="43"/>
+      <c r="AQ43" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -3763,4 +3145,623 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K45"/>
+  <sheetViews>
+    <sheetView topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="10" max="10" width="73.5703125" customWidth="1"/>
+    <col min="11" max="11" width="38.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15" customHeight="1">
+      <c r="A1" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+    </row>
+    <row r="2" spans="1:11" ht="15" customHeight="1">
+      <c r="A2" s="44"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="J2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="14">
+        <v>7</v>
+      </c>
+      <c r="B4" s="15">
+        <v>8</v>
+      </c>
+      <c r="C4" s="16">
+        <v>9</v>
+      </c>
+      <c r="D4" s="15">
+        <v>10</v>
+      </c>
+      <c r="E4" s="16">
+        <v>11</v>
+      </c>
+      <c r="F4" s="15">
+        <v>12</v>
+      </c>
+      <c r="G4" s="17">
+        <v>13</v>
+      </c>
+      <c r="H4" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A5" s="18">
+        <v>14</v>
+      </c>
+      <c r="B5" s="19">
+        <v>15</v>
+      </c>
+      <c r="C5" s="20">
+        <v>16</v>
+      </c>
+      <c r="D5" s="19">
+        <v>17</v>
+      </c>
+      <c r="E5" s="20">
+        <v>18</v>
+      </c>
+      <c r="F5" s="19">
+        <v>19</v>
+      </c>
+      <c r="G5" s="21">
+        <v>20</v>
+      </c>
+      <c r="H5" s="45"/>
+      <c r="J5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="14">
+        <v>21</v>
+      </c>
+      <c r="B6" s="15">
+        <v>22</v>
+      </c>
+      <c r="C6" s="16">
+        <v>23</v>
+      </c>
+      <c r="D6" s="15">
+        <v>24</v>
+      </c>
+      <c r="E6" s="16">
+        <v>25</v>
+      </c>
+      <c r="F6" s="15">
+        <v>26</v>
+      </c>
+      <c r="G6" s="17">
+        <v>27</v>
+      </c>
+      <c r="H6" s="45" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A7" s="18">
+        <v>29</v>
+      </c>
+      <c r="B7" s="19">
+        <v>30</v>
+      </c>
+      <c r="C7" s="20">
+        <v>1</v>
+      </c>
+      <c r="D7" s="19">
+        <v>2</v>
+      </c>
+      <c r="E7" s="20">
+        <v>3</v>
+      </c>
+      <c r="F7" s="19">
+        <v>4</v>
+      </c>
+      <c r="G7" s="21">
+        <v>5</v>
+      </c>
+      <c r="H7" s="45"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A9" s="44"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="14">
+        <v>6</v>
+      </c>
+      <c r="B10" s="15">
+        <v>7</v>
+      </c>
+      <c r="C10" s="16">
+        <v>8</v>
+      </c>
+      <c r="D10" s="15">
+        <v>9</v>
+      </c>
+      <c r="E10" s="16">
+        <v>10</v>
+      </c>
+      <c r="F10" s="15">
+        <v>11</v>
+      </c>
+      <c r="G10" s="17">
+        <v>12</v>
+      </c>
+      <c r="H10" s="45" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A11" s="18">
+        <v>13</v>
+      </c>
+      <c r="B11" s="19">
+        <v>14</v>
+      </c>
+      <c r="C11" s="20">
+        <v>15</v>
+      </c>
+      <c r="D11" s="19">
+        <v>16</v>
+      </c>
+      <c r="E11" s="20">
+        <v>17</v>
+      </c>
+      <c r="F11" s="19">
+        <v>18</v>
+      </c>
+      <c r="G11" s="21">
+        <v>19</v>
+      </c>
+      <c r="H11" s="45"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="44"/>
+    </row>
+    <row r="12" spans="1:11" ht="15" customHeight="1">
+      <c r="A12" s="14">
+        <v>20</v>
+      </c>
+      <c r="B12" s="15">
+        <v>21</v>
+      </c>
+      <c r="C12" s="16">
+        <v>22</v>
+      </c>
+      <c r="D12" s="15">
+        <v>23</v>
+      </c>
+      <c r="E12" s="16">
+        <v>24</v>
+      </c>
+      <c r="F12" s="15">
+        <v>25</v>
+      </c>
+      <c r="G12" s="17">
+        <v>26</v>
+      </c>
+      <c r="H12" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" s="44"/>
+      <c r="J12" s="44"/>
+      <c r="K12" s="44"/>
+    </row>
+    <row r="13" spans="1:11" ht="69.75" customHeight="1" thickBot="1">
+      <c r="A13" s="18">
+        <v>27</v>
+      </c>
+      <c r="B13" s="19">
+        <v>28</v>
+      </c>
+      <c r="C13" s="20">
+        <v>29</v>
+      </c>
+      <c r="D13" s="19">
+        <v>30</v>
+      </c>
+      <c r="E13" s="20">
+        <v>31</v>
+      </c>
+      <c r="F13" s="19">
+        <v>1</v>
+      </c>
+      <c r="G13" s="21">
+        <v>2</v>
+      </c>
+      <c r="H13" s="45"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="8"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="44"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="10"/>
+    </row>
+    <row r="15" spans="1:11" ht="48.75" customHeight="1" thickBot="1">
+      <c r="A15" s="44"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+    </row>
+    <row r="16" spans="1:11" ht="75" customHeight="1" thickBot="1">
+      <c r="A16" s="4">
+        <v>3</v>
+      </c>
+      <c r="B16" s="5">
+        <v>4</v>
+      </c>
+      <c r="C16" s="6">
+        <v>5</v>
+      </c>
+      <c r="D16" s="5">
+        <v>6</v>
+      </c>
+      <c r="E16" s="6">
+        <v>7</v>
+      </c>
+      <c r="F16" s="5">
+        <v>8</v>
+      </c>
+      <c r="G16" s="7">
+        <v>9</v>
+      </c>
+      <c r="H16" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+    </row>
+    <row r="17" spans="9:11">
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" spans="9:11">
+      <c r="I18" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="J18" s="44"/>
+      <c r="K18" s="44"/>
+    </row>
+    <row r="19" spans="9:11">
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
+      <c r="K19" s="44"/>
+    </row>
+    <row r="20" spans="9:11" ht="60">
+      <c r="I20" s="9">
+        <v>1</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="9:11">
+      <c r="I21" s="9">
+        <v>2</v>
+      </c>
+      <c r="J21" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K21" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="9:11">
+      <c r="I22" s="9">
+        <v>3</v>
+      </c>
+      <c r="J22" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="9:11">
+      <c r="I23" s="9">
+        <v>4</v>
+      </c>
+      <c r="J23" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="K23" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="9:11">
+      <c r="I24" s="9">
+        <v>5</v>
+      </c>
+      <c r="J24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="9:11">
+      <c r="I25" s="44" t="s">
+        <v>29</v>
+      </c>
+      <c r="J25" s="44"/>
+      <c r="K25" s="44"/>
+    </row>
+    <row r="26" spans="9:11">
+      <c r="I26" s="44"/>
+      <c r="J26" s="44"/>
+      <c r="K26" s="44"/>
+    </row>
+    <row r="27" spans="9:11">
+      <c r="I27" s="9">
+        <v>1</v>
+      </c>
+      <c r="J27" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="K27" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="9:11">
+      <c r="I28" s="9">
+        <v>2</v>
+      </c>
+      <c r="J28" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="K28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="9:11">
+      <c r="I29" s="9">
+        <v>3</v>
+      </c>
+      <c r="J29" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="K29" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="9:11">
+      <c r="I30" s="9">
+        <v>4</v>
+      </c>
+      <c r="J30" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="K30" s="9"/>
+    </row>
+    <row r="31" spans="9:11">
+      <c r="I31" s="9">
+        <v>5</v>
+      </c>
+      <c r="J31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="9:11">
+      <c r="I32" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="J32" s="44"/>
+      <c r="K32" s="44"/>
+    </row>
+    <row r="33" spans="9:11">
+      <c r="I33" s="44"/>
+      <c r="J33" s="44"/>
+      <c r="K33" s="44"/>
+    </row>
+    <row r="34" spans="9:11">
+      <c r="I34" s="9">
+        <v>1</v>
+      </c>
+      <c r="J34" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="K34" s="8"/>
+    </row>
+    <row r="35" spans="9:11">
+      <c r="I35" s="9">
+        <v>2</v>
+      </c>
+      <c r="J35" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="9:11">
+      <c r="I36" s="9">
+        <v>3</v>
+      </c>
+      <c r="J36" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="K36" s="9"/>
+    </row>
+    <row r="37" spans="9:11">
+      <c r="I37" s="9">
+        <v>4</v>
+      </c>
+      <c r="J37" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="K37" s="9"/>
+    </row>
+    <row r="38" spans="9:11">
+      <c r="I38" s="9">
+        <v>5</v>
+      </c>
+      <c r="J38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="9:11">
+      <c r="I39" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="J39" s="44"/>
+      <c r="K39" s="44"/>
+    </row>
+    <row r="40" spans="9:11">
+      <c r="I40" s="44"/>
+      <c r="J40" s="44"/>
+      <c r="K40" s="44"/>
+    </row>
+    <row r="41" spans="9:11">
+      <c r="I41" s="9">
+        <v>1</v>
+      </c>
+      <c r="J41" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="K41" s="8"/>
+    </row>
+    <row r="42" spans="9:11">
+      <c r="I42" s="9">
+        <v>2</v>
+      </c>
+      <c r="J42" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="9:11">
+      <c r="I43" s="9">
+        <v>3</v>
+      </c>
+      <c r="J43" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="K43" s="9"/>
+    </row>
+    <row r="44" spans="9:11">
+      <c r="I44" s="9">
+        <v>4</v>
+      </c>
+      <c r="J44" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="K44" s="9"/>
+    </row>
+    <row r="45" spans="9:11">
+      <c r="I45" s="9">
+        <v>5</v>
+      </c>
+      <c r="J45" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="I11:K12"/>
+    <mergeCell ref="I18:K19"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="A8:G9"/>
+    <mergeCell ref="I39:K40"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="A14:G15"/>
+    <mergeCell ref="I25:K26"/>
+    <mergeCell ref="I32:K33"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="K21" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>